<commit_message>
Add final test data results
</commit_message>
<xml_diff>
--- a/Confusion_Matrix.xlsx
+++ b/Confusion_Matrix.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/payoj/Documents/Spring 2018/Independent Study (ClearEarth)/data/bio/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/payoj/Documents/Spring 2018/Independent Study (ClearEarth)/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="BIOLOGY" sheetId="1" r:id="rId1"/>
-    <sheet name="GEOLOGY" sheetId="2" r:id="rId2"/>
+    <sheet name="Bio_test" sheetId="3" r:id="rId2"/>
+    <sheet name="GEOLOGY" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="33">
   <si>
     <t>BIOTIC_ENTITY-B</t>
   </si>
@@ -133,7 +134,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -201,8 +202,21 @@
       <color theme="5" tint="-0.249977111117893"/>
       <name val="Calibri (Body)"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFC65911"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -213,6 +227,12 @@
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBDD7EE"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -240,7 +260,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -258,8 +278,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -271,8 +295,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -281,6 +307,8 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -289,6 +317,8 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -567,7 +597,7 @@
   <dimension ref="A2:T24"/>
   <sheetViews>
     <sheetView zoomScale="74" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="A5" sqref="A5:A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1841,10 +1871,1278 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:T22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="34.5" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="4" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="6" max="6" width="16.5" customWidth="1"/>
+    <col min="7" max="7" width="17" customWidth="1"/>
+    <col min="12" max="12" width="11.83203125" customWidth="1"/>
+    <col min="13" max="13" width="11.33203125" customWidth="1"/>
+    <col min="18" max="18" width="17.5" customWidth="1"/>
+    <col min="19" max="19" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A2" s="11"/>
+      <c r="B2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="P2" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q2" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="R2" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="S2" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="T2" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A3" s="7"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>554</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>31</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>24</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>7</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
+      </c>
+      <c r="T4">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>62</v>
+      </c>
+      <c r="C5">
+        <v>58</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>3</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>1</v>
+      </c>
+      <c r="T5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>378</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>4</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>3</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>29</v>
+      </c>
+      <c r="E7">
+        <v>10</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>2</v>
+      </c>
+      <c r="T7">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>165</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>6</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>6</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>16</v>
+      </c>
+      <c r="G9">
+        <v>122</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>2</v>
+      </c>
+      <c r="S9">
+        <v>2</v>
+      </c>
+      <c r="T9">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>5</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <v>16</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>21</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>70</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>3</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>6</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>1</v>
+      </c>
+      <c r="T13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>2</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A17" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A18" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
+      </c>
+      <c r="T18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A19" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <v>0</v>
+      </c>
+      <c r="T19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A20" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>2</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20">
+        <v>35</v>
+      </c>
+      <c r="S20">
+        <v>0</v>
+      </c>
+      <c r="T20">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A21" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <v>6</v>
+      </c>
+      <c r="S21">
+        <v>1</v>
+      </c>
+      <c r="T21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A22" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22">
+        <v>11</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
+      </c>
+      <c r="D22">
+        <v>45</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>13</v>
+      </c>
+      <c r="G22">
+        <v>5</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>6</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>2</v>
+      </c>
+      <c r="Q22">
+        <v>0</v>
+      </c>
+      <c r="R22">
+        <v>4</v>
+      </c>
+      <c r="S22">
+        <v>1</v>
+      </c>
+      <c r="T22">
+        <v>4230</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:T25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6:J7"/>
+    <sheetView zoomScale="95" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>